<commit_message>
Update EOMP 3 Login - Khi đăng nhập bằng email vanlang => tự động lên giảng viên => Phải nhập đúng họ tên + mã + dùng chính xác email của bản thân - Khi đăng nhập bằng gmail => cần kích hoạt => Chỉ cần nhập họ tên mà tồn tại trên hệ thống => xóa bỏ form mã gv như Trung Po đưa ra ý kiến - Chỉ có thể đăng nhập với các email sau : @gmail - @vanlanguni.vn - vlu.edu.vn. Các email còn lại sẽ thông báo email bị sai
Danh sách giảng viên
- Hiển thị trường thông tin email
- Thay đổi template khi import -> thêm email
- Có thể chỉnh sửa email
- Khi không có dữ liệu => hiển thị không có

Phân quyền
- Khi không có dữ liệu => hiển thị không có
</commit_message>
<xml_diff>
--- a/CAPTeam14/Doc/DSGiangVien.xlsx
+++ b/CAPTeam14/Doc/DSGiangVien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choco\Desktop\code final\CAPTeam14\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\choco\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30A7994-587B-449F-A40B-BBE9AA57EDD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5807FD3-DFEA-4D1C-B9FD-95EF0DF74C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3380" yWindow="3380" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mã GV</t>
   </si>
@@ -42,112 +42,7 @@
     <t>Loại GV</t>
   </si>
   <si>
-    <t>0300139</t>
-  </si>
-  <si>
-    <t>Bùi Minh Phụng</t>
-  </si>
-  <si>
-    <t>06/03/1976</t>
-  </si>
-  <si>
-    <t>Khoa Công nghệ thông tin</t>
-  </si>
-  <si>
-    <t>Cơ hữu</t>
-  </si>
-  <si>
-    <t>0300145</t>
-  </si>
-  <si>
-    <t>Nguyễn Thế Quang</t>
-  </si>
-  <si>
-    <t>05/01/1978</t>
-  </si>
-  <si>
-    <t>DH00403</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Nguyệt Quế</t>
-  </si>
-  <si>
-    <t>30/04/1984</t>
-  </si>
-  <si>
-    <t>DH00404</t>
-  </si>
-  <si>
-    <t>Hồ Văn Quí</t>
-  </si>
-  <si>
-    <t>12/10/1985</t>
-  </si>
-  <si>
-    <t>16T0777</t>
-  </si>
-  <si>
-    <t>Nguyễn Hữu Quốc</t>
-  </si>
-  <si>
-    <t>23/10/1971</t>
-  </si>
-  <si>
-    <t>DH00405</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Quý</t>
-  </si>
-  <si>
-    <t>15/11/1989</t>
-  </si>
-  <si>
-    <t>Nguyễn Thị Quyên</t>
-  </si>
-  <si>
-    <t>10/02/1982</t>
-  </si>
-  <si>
-    <t>DH00406</t>
-  </si>
-  <si>
-    <t>Ngô Quang Quyền</t>
-  </si>
-  <si>
-    <t>15/10/1985</t>
-  </si>
-  <si>
-    <t>DH00407</t>
-  </si>
-  <si>
-    <t>Trần Ngọc Hải Sơn</t>
-  </si>
-  <si>
-    <t>20/03/1977</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Tân</t>
-  </si>
-  <si>
-    <t>25/02/1989</t>
-  </si>
-  <si>
-    <t>DH00408</t>
-  </si>
-  <si>
-    <t>Đinh Công Thắng</t>
-  </si>
-  <si>
-    <t>17/09/1987</t>
-  </si>
-  <si>
-    <t>12T0624</t>
-  </si>
-  <si>
-    <t>Trần Công Thanh</t>
-  </si>
-  <si>
-    <t>12/02/1985</t>
+    <t>Email</t>
   </si>
 </sst>
 </file>
@@ -215,17 +110,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="61"/>
+        <color indexed="63"/>
       </left>
       <right style="thin">
-        <color indexed="61"/>
+        <color indexed="63"/>
       </right>
-      <top style="thin">
-        <color indexed="61"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="61"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -233,16 +124,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -525,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A2D47B5-BF34-402E-8DBB-6CF803DDA4F1}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="F3" sqref="A2:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,7 +424,7 @@
     <col min="1" max="5" width="23.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -552,209 +440,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
-        <v>2001329</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A11" s="2">
-        <v>2001366</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="20" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>